<commit_message>
Fixed round4 sample_info pre-sequencing summary excel sheet
Co-authored-by: Kristen Maynard <Kristen.Maynard@libd.org>
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/Visium_DLPFC_all4rounds_manually_merged.xlsx
+++ b/raw-data/sample_info/Visium_DLPFC_all4rounds_manually_merged.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leocollado/Dropbox/Code/spatialDLPFC/raw-data/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5420C7DB-7243-6C4E-95DD-40190EAFA708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1236EFFE-11B6-F44D-8F8F-5DED1A70A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19480" yWindow="3680" windowWidth="27640" windowHeight="16940" xr2:uid="{B66B734A-5F93-044A-AE59-DEF2AFBEF472}"/>
+    <workbookView xWindow="3040" yWindow="1600" windowWidth="42160" windowHeight="22460" xr2:uid="{B66B734A-5F93-044A-AE59-DEF2AFBEF472}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC59FE4-AE3F-0C46-876D-E97BC7D336BD}">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2340,11 +2340,11 @@
         <v>9990</v>
       </c>
       <c r="Q14" s="15">
-        <f>(P14*40)/1000</f>
+        <f t="shared" ref="Q14:Q19" si="3">(P14*40)/1000</f>
         <v>399.6</v>
       </c>
       <c r="R14" s="15">
-        <f>Q14/4</f>
+        <f t="shared" ref="R14:R19" si="4">Q14/4</f>
         <v>99.9</v>
       </c>
       <c r="S14" s="10">
@@ -2372,7 +2372,7 @@
         <v>70</v>
       </c>
       <c r="AA14" s="18">
-        <f>(5000*(Z14/100))*50000</f>
+        <f t="shared" ref="AA14:AA19" si="5">(5000*(Z14/100))*50000</f>
         <v>175000000</v>
       </c>
     </row>
@@ -2417,11 +2417,11 @@
         <v>9533</v>
       </c>
       <c r="Q15" s="15">
-        <f>(P15*40)/1000</f>
+        <f t="shared" si="3"/>
         <v>381.32</v>
       </c>
       <c r="R15" s="15">
-        <f>Q15/4</f>
+        <f t="shared" si="4"/>
         <v>95.33</v>
       </c>
       <c r="S15" s="10">
@@ -2449,7 +2449,7 @@
         <v>30</v>
       </c>
       <c r="AA15" s="18">
-        <f>(5000*(Z15/100))*50000</f>
+        <f t="shared" si="5"/>
         <v>75000000</v>
       </c>
     </row>
@@ -2494,11 +2494,11 @@
         <v>15929</v>
       </c>
       <c r="Q16" s="15">
-        <f>(P16*40)/1000</f>
+        <f t="shared" si="3"/>
         <v>637.16</v>
       </c>
       <c r="R16" s="15">
-        <f>Q16/4</f>
+        <f t="shared" si="4"/>
         <v>159.29</v>
       </c>
       <c r="S16" s="10">
@@ -2526,7 +2526,7 @@
         <v>95</v>
       </c>
       <c r="AA16" s="18">
-        <f>(5000*(Z16/100))*50000</f>
+        <f t="shared" si="5"/>
         <v>237500000</v>
       </c>
     </row>
@@ -2571,11 +2571,11 @@
         <v>14867</v>
       </c>
       <c r="Q17" s="15">
-        <f>(P17*40)/1000</f>
+        <f t="shared" si="3"/>
         <v>594.67999999999995</v>
       </c>
       <c r="R17" s="15">
-        <f>Q17/4</f>
+        <f t="shared" si="4"/>
         <v>148.66999999999999</v>
       </c>
       <c r="S17" s="10">
@@ -2603,7 +2603,7 @@
         <v>70</v>
       </c>
       <c r="AA17" s="18">
-        <f>(5000*(Z17/100))*50000</f>
+        <f t="shared" si="5"/>
         <v>175000000</v>
       </c>
     </row>
@@ -2648,11 +2648,11 @@
         <v>18920</v>
       </c>
       <c r="Q18" s="15">
-        <f>(P18*40)/1000</f>
+        <f t="shared" si="3"/>
         <v>756.8</v>
       </c>
       <c r="R18" s="15">
-        <f>Q18/4</f>
+        <f t="shared" si="4"/>
         <v>189.2</v>
       </c>
       <c r="S18" s="10">
@@ -2680,7 +2680,7 @@
         <v>60</v>
       </c>
       <c r="AA18" s="18">
-        <f>(5000*(Z18/100))*50000</f>
+        <f t="shared" si="5"/>
         <v>150000000</v>
       </c>
     </row>
@@ -2722,11 +2722,11 @@
         <v>13992</v>
       </c>
       <c r="Q19" s="15">
-        <f>(P19*40)/1000</f>
+        <f t="shared" si="3"/>
         <v>559.67999999999995</v>
       </c>
       <c r="R19" s="15">
-        <f>Q19/4</f>
+        <f t="shared" si="4"/>
         <v>139.91999999999999</v>
       </c>
       <c r="S19" s="10">
@@ -2754,7 +2754,7 @@
         <v>50</v>
       </c>
       <c r="AA19" s="18">
-        <f>(5000*(Z19/100))*50000</f>
+        <f t="shared" si="5"/>
         <v>125000000</v>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
         <v>0.8</v>
       </c>
       <c r="AA21">
-        <f t="shared" ref="AA21:AA31" si="3">5000*Z21*50000</f>
+        <f t="shared" ref="AA21:AA31" si="6">5000*Z21*50000</f>
         <v>200000000</v>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
         <v>0.8</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
         <v>0.8</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
         <v>0.8</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6">
-        <f t="shared" ref="R25:R31" si="4">(P25/1000)*10</f>
+        <f t="shared" ref="R25:R31" si="7">(P25/1000)*10</f>
         <v>231.14999999999998</v>
       </c>
       <c r="S25" s="4">
@@ -3188,7 +3188,7 @@
         <v>0.8</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="Q26" s="6"/>
       <c r="R26" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>351.70000000000005</v>
       </c>
       <c r="S26" s="4">
@@ -3267,7 +3267,7 @@
         <v>0.8</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="Q27" s="6"/>
       <c r="R27" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>309.54999999999995</v>
       </c>
       <c r="S27" s="4">
@@ -3343,7 +3343,7 @@
         <v>0.8</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="Q28" s="6"/>
       <c r="R28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>309.14999999999998</v>
       </c>
       <c r="S28" s="4">
@@ -3419,7 +3419,7 @@
         <v>0.8</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="Q29" s="6"/>
       <c r="R29" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>294.89999999999998</v>
       </c>
       <c r="S29" s="4">
@@ -3495,7 +3495,7 @@
         <v>0.8</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="Q30" s="6"/>
       <c r="R30" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>273.95</v>
       </c>
       <c r="S30" s="4">
@@ -3571,7 +3571,7 @@
         <v>0.8</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="Q31" s="6"/>
       <c r="R31" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>518.25</v>
       </c>
       <c r="S31" s="4">
@@ -3650,7 +3650,7 @@
         <v>0.8</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>200000000</v>
       </c>
     </row>
@@ -3696,12 +3696,10 @@
         <v>66.260000000000005</v>
       </c>
       <c r="Q32" s="6">
-        <f>P32*40</f>
-        <v>2650.4</v>
+        <v>26.504000000000001</v>
       </c>
       <c r="R32" s="6">
-        <f>Q32/4</f>
-        <v>662.6</v>
+        <v>6.6260000000000003</v>
       </c>
       <c r="S32" s="4">
         <v>18</v>
@@ -3768,12 +3766,10 @@
         <v>1154.6400000000001</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" ref="Q33:Q35" si="5">P33*40</f>
-        <v>46185.600000000006</v>
+        <v>461.85600000000005</v>
       </c>
       <c r="R33" s="6">
-        <f t="shared" ref="R33:R35" si="6">Q33/4</f>
-        <v>11546.400000000001</v>
+        <v>115.46400000000001</v>
       </c>
       <c r="S33" s="4">
         <v>15</v>
@@ -3796,7 +3792,7 @@
         <v>85</v>
       </c>
       <c r="AA33">
-        <f t="shared" ref="AA33:AA35" si="7">((Z33/100)*5000)*75000</f>
+        <f t="shared" ref="AA33:AA35" si="8">((Z33/100)*5000)*75000</f>
         <v>318750000</v>
       </c>
     </row>
@@ -3842,12 +3838,10 @@
         <v>1360.4</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" si="5"/>
-        <v>54416</v>
+        <v>544.16</v>
       </c>
       <c r="R34" s="6">
-        <f t="shared" si="6"/>
-        <v>13604</v>
+        <v>136.04</v>
       </c>
       <c r="S34" s="4">
         <v>15</v>
@@ -3870,7 +3864,7 @@
         <v>80</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300000000</v>
       </c>
     </row>
@@ -3916,12 +3910,10 @@
         <v>256.01</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" si="5"/>
-        <v>10240.4</v>
+        <v>102.404</v>
       </c>
       <c r="R35" s="6">
-        <f t="shared" si="6"/>
-        <v>2560.1</v>
+        <v>25.600999999999999</v>
       </c>
       <c r="S35" s="4">
         <v>18</v>
@@ -3944,7 +3936,7 @@
         <v>75</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>281250000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix units of 'Est Read Pairs' to be in millions like other sheets. Only for round 1
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/Visium_DLPFC_all4rounds_manually_merged.xlsx
+++ b/raw-data/sample_info/Visium_DLPFC_all4rounds_manually_merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leocollado/Dropbox/Code/spatialDLPFC/raw-data/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1236EFFE-11B6-F44D-8F8F-5DED1A70A309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85307A39-547D-254A-8AEF-7037957FA898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1600" windowWidth="42160" windowHeight="22460" xr2:uid="{B66B734A-5F93-044A-AE59-DEF2AFBEF472}"/>
+    <workbookView xWindow="55240" yWindow="500" windowWidth="42160" windowHeight="22460" xr2:uid="{B66B734A-5F93-044A-AE59-DEF2AFBEF472}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,9 +612,6 @@
     <t>Ave frag length library</t>
   </si>
   <si>
-    <t xml:space="preserve">Est Read Pairs (million) </t>
-  </si>
-  <si>
     <t>V19B23-075</t>
   </si>
   <si>
@@ -766,6 +763,9 @@
   </si>
   <si>
     <t>GACAGAGCCG</t>
+  </si>
+  <si>
+    <t>Est Read Pairs</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1356,7 @@
         <v>17</v>
       </c>
       <c r="AA1" s="13" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -1385,7 +1385,7 @@
         <v>46</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>20</v>
@@ -1418,23 +1418,23 @@
         <v>13358.599999999999</v>
       </c>
       <c r="V2" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="W2" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="18" t="s">
+      <c r="X2" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="18" t="s">
+      <c r="Y2" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="Y2" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="Z2" s="10">
         <v>0.75</v>
       </c>
       <c r="AA2" s="10">
-        <f>Z2*5000*50</f>
-        <v>187500</v>
+        <f>Z2*5000*50000</f>
+        <v>187500000</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -1463,7 +1463,7 @@
         <v>47</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>25</v>
@@ -1496,23 +1496,23 @@
         <v>29076</v>
       </c>
       <c r="V3" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="W3" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="Y3" s="18" t="s">
         <v>185</v>
-      </c>
-      <c r="Y3" s="18" t="s">
-        <v>186</v>
       </c>
       <c r="Z3" s="10">
         <v>0.7</v>
       </c>
       <c r="AA3" s="10">
-        <f t="shared" ref="AA3:AA13" si="2">Z3*5000*50</f>
-        <v>175000</v>
+        <f t="shared" ref="AA3:AA13" si="2">Z3*5000*50000</f>
+        <v>175000000</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -1544,7 +1544,7 @@
         <v>48</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>30</v>
@@ -1577,23 +1577,23 @@
         <v>13571.6</v>
       </c>
       <c r="V4" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="W4" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="W4" s="18" t="s">
+      <c r="X4" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="Y4" s="18" t="s">
         <v>189</v>
-      </c>
-      <c r="Y4" s="18" t="s">
-        <v>190</v>
       </c>
       <c r="Z4" s="10">
         <v>0.75</v>
       </c>
       <c r="AA4" s="10">
         <f t="shared" si="2"/>
-        <v>187500</v>
+        <v>187500000</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -1622,7 +1622,7 @@
         <v>49</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>35</v>
@@ -1655,23 +1655,23 @@
         <v>46616</v>
       </c>
       <c r="V5" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="W5" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="X5" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="Y5" s="18" t="s">
         <v>193</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>194</v>
       </c>
       <c r="Z5" s="10">
         <v>0.9</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" si="2"/>
-        <v>225000</v>
+        <v>225000000</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
@@ -1703,7 +1703,7 @@
         <v>50</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>20</v>
@@ -1735,23 +1735,23 @@
         <v>18362.919999999998</v>
       </c>
       <c r="V6" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="W6" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="W6" s="18" t="s">
+      <c r="X6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="Y6" s="18" t="s">
         <v>198</v>
-      </c>
-      <c r="Y6" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="Z6" s="10">
         <v>0.8</v>
       </c>
       <c r="AA6" s="10">
         <f t="shared" si="2"/>
-        <v>200000</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
         <v>51</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>25</v>
@@ -1812,23 +1812,23 @@
         <v>21018.79</v>
       </c>
       <c r="V7" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="W7" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="W7" s="18" t="s">
+      <c r="X7" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="X7" s="18" t="s">
+      <c r="Y7" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="Y7" s="18" t="s">
-        <v>203</v>
       </c>
       <c r="Z7" s="10">
         <v>0.6</v>
       </c>
       <c r="AA7" s="10">
         <f t="shared" si="2"/>
-        <v>150000</v>
+        <v>150000000</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -1860,7 +1860,7 @@
         <v>52</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>30</v>
@@ -1892,23 +1892,23 @@
         <v>16002.97</v>
       </c>
       <c r="V8" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="W8" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="W8" s="18" t="s">
+      <c r="X8" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="Y8" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="Y8" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="Z8" s="10">
         <v>0.7</v>
       </c>
       <c r="AA8" s="10">
         <f t="shared" si="2"/>
-        <v>175000</v>
+        <v>175000000</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
@@ -1940,7 +1940,7 @@
         <v>53</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>35</v>
@@ -1972,23 +1972,23 @@
         <v>30634.04</v>
       </c>
       <c r="V9" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="W9" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="W9" s="18" t="s">
+      <c r="X9" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="X9" s="18" t="s">
+      <c r="Y9" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="Y9" s="18" t="s">
-        <v>211</v>
       </c>
       <c r="Z9" s="10">
         <v>0.85</v>
       </c>
       <c r="AA9" s="10">
         <f t="shared" si="2"/>
-        <v>212500</v>
+        <v>212500000</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -2017,7 +2017,7 @@
         <v>54</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>20</v>
@@ -2049,23 +2049,23 @@
         <v>17508.96</v>
       </c>
       <c r="V10" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="W10" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="W10" s="18" t="s">
+      <c r="X10" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="X10" s="18" t="s">
+      <c r="Y10" s="18" t="s">
         <v>215</v>
-      </c>
-      <c r="Y10" s="18" t="s">
-        <v>216</v>
       </c>
       <c r="Z10" s="10">
         <v>0.6</v>
       </c>
       <c r="AA10" s="10">
         <f t="shared" si="2"/>
-        <v>150000</v>
+        <v>150000000</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
@@ -2094,7 +2094,7 @@
         <v>55</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>25</v>
@@ -2126,23 +2126,23 @@
         <v>17152.79</v>
       </c>
       <c r="V11" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="W11" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="W11" s="18" t="s">
+      <c r="X11" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="Y11" s="18" t="s">
         <v>219</v>
-      </c>
-      <c r="Y11" s="18" t="s">
-        <v>220</v>
       </c>
       <c r="Z11" s="10">
         <v>0.8</v>
       </c>
       <c r="AA11" s="10">
         <f t="shared" si="2"/>
-        <v>200000</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
@@ -2171,7 +2171,7 @@
         <v>56</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>30</v>
@@ -2203,23 +2203,23 @@
         <v>19004.28</v>
       </c>
       <c r="V12" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="W12" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="W12" s="18" t="s">
+      <c r="X12" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="X12" s="18" t="s">
+      <c r="Y12" s="18" t="s">
         <v>223</v>
-      </c>
-      <c r="Y12" s="18" t="s">
-        <v>224</v>
       </c>
       <c r="Z12" s="10">
         <v>0.65</v>
       </c>
       <c r="AA12" s="10">
         <f t="shared" si="2"/>
-        <v>162500</v>
+        <v>162500000</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -2248,7 +2248,7 @@
         <v>57</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>35</v>
@@ -2280,23 +2280,23 @@
         <v>16301.68</v>
       </c>
       <c r="V13" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="W13" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="W13" s="18" t="s">
+      <c r="X13" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="X13" s="18" t="s">
+      <c r="Y13" s="18" t="s">
         <v>227</v>
-      </c>
-      <c r="Y13" s="18" t="s">
-        <v>228</v>
       </c>
       <c r="Z13" s="10">
         <v>0.9</v>
       </c>
       <c r="AA13" s="10">
         <f t="shared" si="2"/>
-        <v>225000</v>
+        <v>225000000</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>